<commit_message>
updated case list formatting for initial tables
</commit_message>
<xml_diff>
--- a/case_list.xlsx
+++ b/case_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="684" yWindow="360" windowWidth="15984" windowHeight="6108"/>
+    <workbookView xWindow="680" yWindow="360" windowWidth="15980" windowHeight="6110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
   <si>
     <t>F0</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>Estimation</t>
-  </si>
-  <si>
-    <t>Small bin width</t>
-  </si>
-  <si>
-    <t>Broad bin width</t>
   </si>
   <si>
     <t>I0</t>
@@ -144,9 +138,6 @@
     <t>External case, using the change_em_binning function</t>
   </si>
   <si>
-    <t>Medium bin width</t>
-  </si>
-  <si>
     <t>B3</t>
   </si>
   <si>
@@ -228,30 +219,12 @@
     <t># of data bins</t>
   </si>
   <si>
-    <t># of pop bins</t>
-  </si>
-  <si>
-    <t>bin width</t>
-  </si>
-  <si>
-    <t>1cm binning base case</t>
-  </si>
-  <si>
     <t>Set 1cm OM bins and min/max</t>
   </si>
   <si>
-    <t>Linf</t>
-  </si>
-  <si>
     <t>Model setup</t>
   </si>
   <si>
-    <t>min pop bin</t>
-  </si>
-  <si>
-    <t>max pop bin</t>
-  </si>
-  <si>
     <t>min data bin</t>
   </si>
   <si>
@@ -271,6 +244,55 @@
   </si>
   <si>
     <t>Pop bins= 1cm &amp; robustification constant = 0.5</t>
+  </si>
+  <si>
+    <t>Min Bin (cm)</t>
+  </si>
+  <si>
+    <t>Max Bin (cm)</t>
+  </si>
+  <si>
+    <t>flatfish</t>
+  </si>
+  <si>
+    <t>rockfish</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>∞</t>
+    </r>
+  </si>
+  <si>
+    <t>Base case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium </t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Bin Width (cm)</t>
+  </si>
+  <si>
+    <t># of bins</t>
+  </si>
+  <si>
+    <t>bin width: Linf</t>
   </si>
 </sst>
 </file>
@@ -280,7 +302,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +366,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -365,7 +403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -538,12 +576,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -618,7 +671,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,6 +714,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -742,7 +827,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$10</c:f>
+              <c:f>Sheet1!$J$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -765,7 +850,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$11:$M$15</c:f>
+              <c:f>Sheet1!$J$11:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -794,11 +879,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$10</c:f>
+              <c:f>Sheet1!$K$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>fla</c:v>
+                  <c:v>flatfish</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -817,7 +902,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$11:$N$15</c:f>
+              <c:f>Sheet1!$K$11:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -846,11 +931,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$10</c:f>
+              <c:f>Sheet1!$L$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>yel</c:v>
+                  <c:v>rockfish</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -869,7 +954,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$11:$O$15</c:f>
+              <c:f>Sheet1!$L$11:$L$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -903,11 +988,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84130816"/>
-        <c:axId val="84354176"/>
+        <c:axId val="122877824"/>
+        <c:axId val="122879360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84130816"/>
+        <c:axId val="122877824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -949,7 +1034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84354176"/>
+        <c:crossAx val="122879360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -957,7 +1042,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84354176"/>
+        <c:axId val="122879360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +1093,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84130816"/>
+        <c:crossAx val="122877824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1969,204 +2054,188 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L9" sqref="C9:L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="36.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.45" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.45" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C4" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>72</v>
+      <c r="E4" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>62</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B5" s="48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B5" s="47" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="19">
         <v>8</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="59">
         <v>200</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="54">
+        <v>132</v>
+      </c>
+      <c r="F5" s="19">
         <f>C5</f>
         <v>8</v>
       </c>
-      <c r="F5" s="14">
-        <f t="shared" ref="F5:F7" si="0">D5</f>
+      <c r="G5" s="14">
+        <f>D5</f>
         <v>200</v>
       </c>
-      <c r="G5" s="14">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B6" s="49" t="s">
-        <v>4</v>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B6" s="48" t="s">
+        <v>71</v>
       </c>
       <c r="C6" s="20">
         <v>2</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="60">
         <v>102</v>
       </c>
-      <c r="E6" s="20">
-        <f t="shared" ref="E6:E7" si="1">C6</f>
+      <c r="E6" s="56">
+        <v>47.424500000000002</v>
+      </c>
+      <c r="F6" s="20">
+        <f>C6</f>
         <v>2</v>
       </c>
-      <c r="F6" s="16">
-        <f t="shared" si="0"/>
+      <c r="G6" s="16">
+        <f>D6</f>
         <v>102</v>
       </c>
-      <c r="G6" s="23">
-        <v>47.424500000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B7" s="50" t="s">
-        <v>7</v>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B7" s="49" t="s">
+        <v>72</v>
       </c>
       <c r="C7" s="21">
         <v>10</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="61">
         <v>106</v>
       </c>
-      <c r="E7" s="21">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="F7" s="18">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="G7" s="18">
+      <c r="E7" s="55">
         <v>62</v>
       </c>
-      <c r="I7">
+      <c r="F7" s="21">
         <f>C7</f>
         <v>10</v>
       </c>
-      <c r="J7">
-        <f>I7+24</f>
-        <v>34</v>
-      </c>
-      <c r="K7" s="2">
-        <f t="shared" ref="K7:M7" si="2">J7+24</f>
-        <v>58</v>
-      </c>
-      <c r="L7" s="2">
-        <f t="shared" si="2"/>
-        <v>82</v>
-      </c>
-      <c r="M7" s="2">
-        <f t="shared" si="2"/>
+      <c r="G7" s="18">
+        <f>D7</f>
         <v>106</v>
       </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="15.45" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B9" s="51" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B9" s="50" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="2"/>
+      <c r="K9" t="s">
+        <v>80</v>
+      </c>
       <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B10" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="40"/>
+      <c r="N9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="39"/>
       <c r="D10" s="32" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="G10" s="32" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="J10" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="33" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="M10" s="32" t="s">
         <v>5</v>
@@ -2178,67 +2247,67 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="38">
+      <c r="C11" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="37">
         <v>1</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="36">
         <v>1</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="36">
         <v>1</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="37">
         <f>($D$5-$C$5)/D11</f>
         <v>192</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="36">
         <f>($D$6-$C$6)/E11</f>
         <v>100</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="36">
         <f>($D$7-$C$7)/F11</f>
         <v>96</v>
       </c>
-      <c r="J11" s="38">
-        <f>($F$5-$E$5)/D11</f>
+      <c r="J11" s="40">
+        <f>D11/$E$5</f>
+        <v>7.575757575757576E-3</v>
+      </c>
+      <c r="K11" s="41">
+        <f>E11/$E$6</f>
+        <v>2.1086147455429156E-2</v>
+      </c>
+      <c r="L11" s="42">
+        <f>F11/$E$7</f>
+        <v>1.6129032258064516E-2</v>
+      </c>
+      <c r="M11" s="37">
+        <f>($G$5-$F$5)/D11</f>
         <v>192</v>
       </c>
-      <c r="K11" s="37">
-        <f>($F$6-$E$6)/E11</f>
+      <c r="N11" s="36">
+        <f>($G$6-$F$6)/E11</f>
         <v>100</v>
       </c>
-      <c r="L11" s="37">
-        <f>($F$7-$E$7)/F11</f>
+      <c r="O11" s="36">
+        <f>($G$7-$F$7)/F11</f>
         <v>96</v>
       </c>
-      <c r="M11" s="41">
-        <f>D11/$G$5</f>
-        <v>7.575757575757576E-3</v>
-      </c>
-      <c r="N11" s="42">
-        <f>E11/$G$6</f>
-        <v>2.1086147455429156E-2</v>
-      </c>
-      <c r="O11" s="43">
-        <f>F11/$G$7</f>
-        <v>1.6129032258064516E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>11</v>
+      <c r="C12" s="63" t="s">
+        <v>77</v>
       </c>
       <c r="D12" s="20">
         <v>2</v>
@@ -2261,38 +2330,38 @@
         <f>($D$7-$C$7)/F12</f>
         <v>48</v>
       </c>
-      <c r="J12" s="20">
-        <f>($F$5-$E$5)/D12</f>
+      <c r="J12" s="43">
+        <f>D12/$E$5</f>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="K12" s="28">
+        <f>E12/$E$6</f>
+        <v>4.2172294910858311E-2</v>
+      </c>
+      <c r="L12" s="29">
+        <f>F12/$E$7</f>
+        <v>3.2258064516129031E-2</v>
+      </c>
+      <c r="M12" s="20">
+        <f>($G$5-$F$5)/D12</f>
         <v>96</v>
       </c>
-      <c r="K12" s="15">
-        <f>($F$6-$E$6)/E12</f>
+      <c r="N12" s="15">
+        <f>($G$6-$F$6)/E12</f>
         <v>50</v>
       </c>
-      <c r="L12" s="15">
-        <f>($F$7-$E$7)/F12</f>
+      <c r="O12" s="15">
+        <f>($G$7-$F$7)/F12</f>
         <v>48</v>
       </c>
-      <c r="M12" s="44">
-        <f>D12/$G$5</f>
-        <v>1.5151515151515152E-2</v>
-      </c>
-      <c r="N12" s="28">
-        <f>E12/$G$6</f>
-        <v>4.2172294910858311E-2</v>
-      </c>
-      <c r="O12" s="29">
-        <f>F12/$G$7</f>
-        <v>3.2258064516129031E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>35</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>76</v>
       </c>
       <c r="D13" s="20">
         <v>4</v>
@@ -2315,37 +2384,37 @@
         <f>($D$7-$C$7)/F13</f>
         <v>24</v>
       </c>
-      <c r="J13" s="20">
-        <f>($F$5-$E$5)/D13</f>
+      <c r="J13" s="43">
+        <f>D13/$E$5</f>
+        <v>3.0303030303030304E-2</v>
+      </c>
+      <c r="K13" s="28">
+        <f>E13/$E$6</f>
+        <v>0.10543073727714578</v>
+      </c>
+      <c r="L13" s="29">
+        <f>F13/$E$7</f>
+        <v>6.4516129032258063E-2</v>
+      </c>
+      <c r="M13" s="20">
+        <f>($G$5-$F$5)/D13</f>
         <v>48</v>
       </c>
-      <c r="K13" s="15">
-        <f>($F$6-$E$6)/E13</f>
+      <c r="N13" s="15">
+        <f>($G$6-$F$6)/E13</f>
         <v>20</v>
       </c>
-      <c r="L13" s="15">
-        <f>($F$7-$E$7)/F13</f>
+      <c r="O13" s="15">
+        <f>($G$7-$F$7)/F13</f>
         <v>24</v>
       </c>
-      <c r="M13" s="44">
-        <f>D13/$G$5</f>
-        <v>3.0303030303030304E-2</v>
-      </c>
-      <c r="N13" s="28">
-        <f>E13/$G$6</f>
-        <v>0.10543073727714578</v>
-      </c>
-      <c r="O13" s="29">
-        <f>F13/$G$7</f>
-        <v>6.4516129032258063E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="C14" s="63" t="s">
+        <v>75</v>
       </c>
       <c r="D14" s="20">
         <v>12</v>
@@ -2368,37 +2437,37 @@
         <f>($D$7-$C$7)/F14</f>
         <v>8</v>
       </c>
-      <c r="J14" s="20">
-        <f>($F$5-$E$5)/D14</f>
+      <c r="J14" s="43">
+        <f>D14/$E$5</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="K14" s="28">
+        <f>E14/$E$6</f>
+        <v>0.21086147455429155</v>
+      </c>
+      <c r="L14" s="29">
+        <f>F14/$E$7</f>
+        <v>0.19354838709677419</v>
+      </c>
+      <c r="M14" s="20">
+        <f>($G$5-$F$5)/D14</f>
         <v>16</v>
       </c>
-      <c r="K14" s="15">
-        <f>($F$6-$E$6)/E14</f>
+      <c r="N14" s="15">
+        <f>($G$6-$F$6)/E14</f>
         <v>10</v>
       </c>
-      <c r="L14" s="15">
-        <f>($F$7-$E$7)/F14</f>
+      <c r="O14" s="15">
+        <f>($G$7-$F$7)/F14</f>
         <v>8</v>
       </c>
-      <c r="M14" s="44">
-        <f>D14/$G$5</f>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="N14" s="28">
-        <f>E14/$G$6</f>
-        <v>0.21086147455429155</v>
-      </c>
-      <c r="O14" s="29">
-        <f>F14/$G$7</f>
-        <v>0.19354838709677419</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>56</v>
       </c>
       <c r="D15" s="21">
         <v>24</v>
@@ -2421,32 +2490,32 @@
         <f>($D$7-$C$7)/F15</f>
         <v>4</v>
       </c>
-      <c r="J15" s="21">
-        <f>($F$5-$E$5)/D15</f>
+      <c r="J15" s="44">
+        <f>D15/$E$5</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="K15" s="30">
+        <f>E15/$E$6</f>
+        <v>0.4217229491085831</v>
+      </c>
+      <c r="L15" s="31">
+        <f>F15/$E$7</f>
+        <v>0.38709677419354838</v>
+      </c>
+      <c r="M15" s="21">
+        <f>($G$5-$F$5)/D15</f>
         <v>8</v>
       </c>
-      <c r="K15" s="17">
-        <f>($F$6-$E$6)/E15</f>
+      <c r="N15" s="17">
+        <f>($G$6-$F$6)/E15</f>
         <v>5</v>
       </c>
-      <c r="L15" s="17">
-        <f>($F$7-$E$7)/F15</f>
+      <c r="O15" s="17">
+        <f>($G$7-$F$7)/F15</f>
         <v>4</v>
       </c>
-      <c r="M15" s="45">
-        <f>D15/$G$5</f>
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="N15" s="30">
-        <f>E15/$G$6</f>
-        <v>0.4217229491085831</v>
-      </c>
-      <c r="O15" s="31">
-        <f>F15/$G$7</f>
-        <v>0.38709677419354838</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -2458,10 +2527,10 @@
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="B17" s="26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -2475,9 +2544,9 @@
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
@@ -2491,9 +2560,9 @@
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="15"/>
@@ -2508,12 +2577,12 @@
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B20" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>66</v>
+    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>60</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -2527,7 +2596,7 @@
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
     </row>
-    <row r="21" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -2540,20 +2609,20 @@
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
     </row>
-    <row r="22" spans="1:14" ht="15.45" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
         <v>0</v>
       </c>
@@ -2561,46 +2630,46 @@
         <v>2</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B25" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="23"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B26" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="23"/>
-    </row>
-    <row r="26" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="B26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>30</v>
-      </c>
       <c r="D26" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="15.45" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -2609,76 +2678,76 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="2" customFormat="1" ht="15.65" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="4" t="s">
+    </row>
+    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="E33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D33" s="3" t="s">
+    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B34" s="51">
+        <v>1</v>
+      </c>
+      <c r="C34" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="3" t="s">
+      <c r="D34" s="52" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="52">
-        <v>1</v>
-      </c>
-      <c r="C34" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53">
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52">
         <v>2</v>
       </c>
-      <c r="H34" s="52">
+      <c r="H34" s="51">
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5">
@@ -2688,19 +2757,19 @@
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G36" s="5">
         <v>2</v>
@@ -2709,37 +2778,37 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="52">
+    <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B37" s="51">
         <v>4</v>
       </c>
-      <c r="C37" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53">
+      <c r="C37" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52">
         <v>2</v>
       </c>
-      <c r="H37" s="52">
+      <c r="H37" s="51">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5">
@@ -2749,19 +2818,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>6</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G39" s="5">
         <v>2</v>
@@ -2770,177 +2839,177 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="52">
+    <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B40" s="51">
         <v>7</v>
       </c>
-      <c r="C40" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53">
+      <c r="C40" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52">
         <v>2</v>
       </c>
-      <c r="H40" s="52" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="52">
+      <c r="H40" s="51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B41" s="51">
         <v>8</v>
       </c>
-      <c r="C41" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="53"/>
-      <c r="F41" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="53">
+      <c r="C41" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="52">
         <v>2</v>
       </c>
-      <c r="H41" s="52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H41" s="51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2">
         <v>0</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2">
         <v>11</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="D47" s="53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2">
         <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48" s="54"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="D48" s="53"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2">
         <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D49" s="54"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="D49" s="53"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2">
         <v>14</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D50" s="54"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="D50" s="53"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2">
         <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D51" s="54"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="D51" s="53"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2">
         <v>21</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D52" s="54" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="D52" s="53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
       <c r="B53" s="2">
         <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D53" s="54"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="D53" s="53"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2">
         <v>23</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D54" s="54"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="D54" s="53"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="2">
         <v>24</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" s="54"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="D55" s="53"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2">
         <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="54"/>
+        <v>68</v>
+      </c>
+      <c r="D56" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
added some  calculations to bin structures
</commit_message>
<xml_diff>
--- a/case_list.xlsx
+++ b/case_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
   <si>
     <t>F0</t>
   </si>
@@ -207,9 +207,6 @@
     <t>B4</t>
   </si>
   <si>
-    <t>Ridiculous</t>
-  </si>
-  <si>
     <t>population bin</t>
   </si>
   <si>
@@ -277,12 +274,6 @@
     <t>Base case</t>
   </si>
   <si>
-    <t xml:space="preserve">Broad </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium </t>
-  </si>
-  <si>
     <t>Small</t>
   </si>
   <si>
@@ -293,6 +284,27 @@
   </si>
   <si>
     <t>bin width: Linf</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>CV_old</t>
+  </si>
+  <si>
+    <t>Linf*3sd</t>
+  </si>
+  <si>
+    <t># sds away</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Extreme</t>
   </si>
 </sst>
 </file>
@@ -596,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -712,41 +724,50 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -988,11 +1009,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="122877824"/>
-        <c:axId val="122879360"/>
+        <c:axId val="116979968"/>
+        <c:axId val="117309440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122877824"/>
+        <c:axId val="116979968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,7 +1055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122879360"/>
+        <c:crossAx val="117309440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1042,7 +1063,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122879360"/>
+        <c:axId val="117309440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,7 +1114,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122877824"/>
+        <c:crossAx val="116979968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2054,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L9" sqref="C9:L15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2066,6 +2087,7 @@
     <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
@@ -2075,33 +2097,45 @@
     </row>
     <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
         <v>57</v>
-      </c>
-      <c r="E3" t="s">
-        <v>58</v>
       </c>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C4" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="57" t="s">
-        <v>73</v>
+      <c r="E4" s="56" t="s">
+        <v>72</v>
       </c>
       <c r="F4" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="34" t="s">
-        <v>63</v>
+      <c r="I4" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="65" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -2111,67 +2145,109 @@
       <c r="C5" s="19">
         <v>8</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="58">
         <v>200</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="53">
         <v>132</v>
       </c>
       <c r="F5" s="19">
-        <f>C5</f>
+        <f t="shared" ref="F5:G7" si="0">C5</f>
         <v>8</v>
       </c>
       <c r="G5" s="14">
-        <f>D5</f>
+        <f t="shared" si="0"/>
         <v>200</v>
+      </c>
+      <c r="I5">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="67">
+        <f>E5*I5</f>
+        <v>13.200000000000001</v>
+      </c>
+      <c r="K5" s="66">
+        <f>E5+3*J5</f>
+        <v>171.6</v>
+      </c>
+      <c r="L5" s="67">
+        <f>(D5-E5)/J5</f>
+        <v>5.1515151515151514</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B6" s="48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="20">
         <v>2</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="59">
         <v>102</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="55">
         <v>47.424500000000002</v>
       </c>
       <c r="F6" s="20">
-        <f>C6</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G6" s="16">
-        <f>D6</f>
+        <f t="shared" si="0"/>
         <v>102</v>
+      </c>
+      <c r="I6">
+        <v>0.2</v>
+      </c>
+      <c r="J6" s="67">
+        <f>E6*I6</f>
+        <v>9.4849000000000014</v>
+      </c>
+      <c r="K6" s="66">
+        <f>E6+3*J6</f>
+        <v>75.879199999999997</v>
+      </c>
+      <c r="L6" s="67">
+        <f>(D6-E6)/J6</f>
+        <v>5.7539352022688686</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" s="49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="21">
         <v>10</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="60">
         <v>106</v>
       </c>
-      <c r="E7" s="55">
+      <c r="E7" s="54">
         <v>62</v>
       </c>
       <c r="F7" s="21">
-        <f>C7</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G7" s="18">
-        <f>D7</f>
+        <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="I7">
+        <v>0.13</v>
+      </c>
+      <c r="J7" s="67">
+        <f>E7*I7</f>
+        <v>8.06</v>
+      </c>
+      <c r="K7" s="66">
+        <f>E7+3*J7</f>
+        <v>86.18</v>
+      </c>
+      <c r="L7" s="67">
+        <f>(D7-E7)/J7</f>
+        <v>5.4590570719602978</v>
+      </c>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
@@ -2188,20 +2264,20 @@
       </c>
       <c r="C9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O9" s="2"/>
     </row>
@@ -2214,28 +2290,28 @@
         <v>5</v>
       </c>
       <c r="E10" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="33" t="s">
         <v>71</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>72</v>
       </c>
       <c r="G10" s="32" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="34" t="s">
         <v>71</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>72</v>
       </c>
       <c r="J10" s="32" t="s">
         <v>5</v>
       </c>
       <c r="K10" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="34" t="s">
         <v>71</v>
-      </c>
-      <c r="L10" s="34" t="s">
-        <v>72</v>
       </c>
       <c r="M10" s="32" t="s">
         <v>5</v>
@@ -2252,8 +2328,8 @@
       <c r="B11" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="62" t="s">
-        <v>74</v>
+      <c r="C11" s="61" t="s">
+        <v>73</v>
       </c>
       <c r="D11" s="37">
         <v>1</v>
@@ -2306,8 +2382,8 @@
       <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="63" t="s">
-        <v>77</v>
+      <c r="C12" s="62" t="s">
+        <v>74</v>
       </c>
       <c r="D12" s="20">
         <v>2</v>
@@ -2360,8 +2436,8 @@
       <c r="B13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="63" t="s">
-        <v>76</v>
+      <c r="C13" s="62" t="s">
+        <v>82</v>
       </c>
       <c r="D13" s="20">
         <v>4</v>
@@ -2413,8 +2489,8 @@
       <c r="B14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="63" t="s">
-        <v>75</v>
+      <c r="C14" s="62" t="s">
+        <v>83</v>
       </c>
       <c r="D14" s="20">
         <v>12</v>
@@ -2466,8 +2542,8 @@
       <c r="B15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="64" t="s">
-        <v>56</v>
+      <c r="C15" s="63" t="s">
+        <v>84</v>
       </c>
       <c r="D15" s="21">
         <v>24</v>
@@ -2582,7 +2658,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -2664,7 +2740,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -2678,7 +2754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="2" customFormat="1" ht="15.65" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>30</v>
       </c>
@@ -2686,7 +2762,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D32" s="4" t="s">
         <v>13</v>
       </c>
@@ -2700,7 +2776,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D33" s="3" t="s">
         <v>17</v>
       </c>
@@ -2717,7 +2793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B34" s="51">
         <v>1</v>
       </c>
@@ -2736,7 +2812,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B35" s="2">
         <v>2</v>
       </c>
@@ -2757,7 +2833,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B36" s="2">
         <v>3</v>
       </c>
@@ -2778,7 +2854,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B37" s="51">
         <v>4</v>
       </c>
@@ -2797,7 +2873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B38" s="2">
         <v>5</v>
       </c>
@@ -2818,7 +2894,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B39" s="2">
         <v>6</v>
       </c>
@@ -2839,7 +2915,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B40" s="51">
         <v>7</v>
       </c>
@@ -2860,7 +2936,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B41" s="51">
         <v>8</v>
       </c>
@@ -2881,7 +2957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="25" t="s">
         <v>38</v>
       </c>
@@ -2891,13 +2967,13 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2">
         <v>0</v>
@@ -2913,9 +2989,9 @@
         <v>11</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="64" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2927,7 +3003,7 @@
       <c r="C48" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="53"/>
+      <c r="D48" s="64"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
@@ -2937,7 +3013,7 @@
       <c r="C49" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="53"/>
+      <c r="D49" s="64"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
@@ -2947,7 +3023,7 @@
       <c r="C50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="53"/>
+      <c r="D50" s="64"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
@@ -2955,9 +3031,9 @@
         <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="53"/>
+        <v>64</v>
+      </c>
+      <c r="D51" s="64"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
@@ -2965,9 +3041,9 @@
         <v>21</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D52" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="64" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2979,7 +3055,7 @@
       <c r="C53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="53"/>
+      <c r="D53" s="64"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
@@ -2989,7 +3065,7 @@
       <c r="C54" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D54" s="53"/>
+      <c r="D54" s="64"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
@@ -2997,9 +3073,9 @@
         <v>24</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D55" s="53"/>
+        <v>66</v>
+      </c>
+      <c r="D55" s="64"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
@@ -3007,9 +3083,9 @@
         <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D56" s="53"/>
+        <v>67</v>
+      </c>
+      <c r="D56" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
prepped to start new runs with updated files
</commit_message>
<xml_diff>
--- a/case_list.xlsx
+++ b/case_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="360" windowWidth="15980" windowHeight="6110"/>
+    <workbookView xWindow="684" yWindow="360" windowWidth="15984" windowHeight="6108"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
   <si>
     <t>F0</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Binning cases</t>
-  </si>
-  <si>
-    <t>yel</t>
   </si>
   <si>
     <t>B0</t>
@@ -213,19 +210,10 @@
     <t>data bin</t>
   </si>
   <si>
-    <t># of data bins</t>
-  </si>
-  <si>
     <t>Set 1cm OM bins and min/max</t>
   </si>
   <si>
     <t>Model setup</t>
-  </si>
-  <si>
-    <t>min data bin</t>
-  </si>
-  <si>
-    <t>max data bin</t>
   </si>
   <si>
     <t>Pop bins= 1cm &amp; tail compression = -1</t>
@@ -306,15 +294,19 @@
   <si>
     <t>Extreme</t>
   </si>
+  <si>
+    <t>% fish above max bin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,6 +386,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -604,11 +603,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -629,19 +629,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -757,22 +748,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -882,13 +875,13 @@
                   <c:v>1.5151515151515152E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0303030303030304E-2</c:v>
+                  <c:v>3.787878787878788E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0909090909090912E-2</c:v>
+                  <c:v>7.575757575757576E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18181818181818182</c:v>
+                  <c:v>0.15151515151515152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -986,13 +979,13 @@
                   <c:v>3.2258064516129031E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4516129032258063E-2</c:v>
+                  <c:v>8.0645161290322578E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19354838709677419</c:v>
+                  <c:v>0.16129032258064516</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38709677419354838</c:v>
+                  <c:v>0.32258064516129031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1009,11 +1002,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116979968"/>
-        <c:axId val="117309440"/>
+        <c:axId val="169551360"/>
+        <c:axId val="169552896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116979968"/>
+        <c:axId val="169551360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="117309440"/>
+        <c:crossAx val="169552896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1063,7 +1056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117309440"/>
+        <c:axId val="169552896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116979968"/>
+        <c:crossAx val="169551360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2075,677 +2068,591 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="18.45" x14ac:dyDescent="0.45">
       <c r="B1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>56</v>
       </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C4" s="32" t="s">
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C4" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B5" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="16">
+        <v>10</v>
+      </c>
+      <c r="D5" s="55">
+        <v>190</v>
+      </c>
+      <c r="E5" s="50">
+        <v>132</v>
+      </c>
+      <c r="G5">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="63">
+        <f>E5*G5</f>
+        <v>13.200000000000001</v>
+      </c>
+      <c r="I5" s="62">
+        <f>E5+3*H5</f>
+        <v>171.6</v>
+      </c>
+      <c r="J5" s="63">
+        <f>(D5-E5)/H5</f>
+        <v>4.3939393939393936</v>
+      </c>
+      <c r="K5" s="65">
+        <f>_xlfn.NORM.DIST(-J5,0,1,TRUE)</f>
+        <v>5.565743045598539E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B6" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="17">
+        <v>2</v>
+      </c>
+      <c r="D6" s="56">
+        <v>102</v>
+      </c>
+      <c r="E6" s="52">
+        <v>47.424500000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="63">
+        <f>E6*G6</f>
+        <v>9.4849000000000014</v>
+      </c>
+      <c r="I6" s="62">
+        <f>E6+3*H6</f>
+        <v>75.879199999999997</v>
+      </c>
+      <c r="J6" s="63">
+        <f>(D6-E6)/H6</f>
+        <v>5.7539352022688686</v>
+      </c>
+      <c r="K6" s="65">
+        <f t="shared" ref="K6:K7" si="0">_xlfn.NORM.DIST(-J6,0,1,TRUE)</f>
+        <v>4.3594793828165778E-9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B7" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="18">
+        <v>10</v>
+      </c>
+      <c r="D7" s="57">
+        <v>110</v>
+      </c>
+      <c r="E7" s="51">
         <v>62</v>
       </c>
-      <c r="I4" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="J4" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="L4" s="65" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="19">
-        <v>8</v>
-      </c>
-      <c r="D5" s="58">
-        <v>200</v>
-      </c>
-      <c r="E5" s="53">
-        <v>132</v>
-      </c>
-      <c r="F5" s="19">
-        <f t="shared" ref="F5:G7" si="0">C5</f>
-        <v>8</v>
-      </c>
-      <c r="G5" s="14">
+      <c r="G7">
+        <v>0.13</v>
+      </c>
+      <c r="H7" s="63">
+        <f>E7*G7</f>
+        <v>8.06</v>
+      </c>
+      <c r="I7" s="62">
+        <f>E7+3*H7</f>
+        <v>86.18</v>
+      </c>
+      <c r="J7" s="63">
+        <f>(D7-E7)/H7</f>
+        <v>5.9553349875930515</v>
+      </c>
+      <c r="K7" s="65">
         <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="I5">
-        <v>0.1</v>
-      </c>
-      <c r="J5" s="67">
-        <f>E5*I5</f>
-        <v>13.200000000000001</v>
-      </c>
-      <c r="K5" s="66">
-        <f>E5+3*J5</f>
-        <v>171.6</v>
-      </c>
-      <c r="L5" s="67">
-        <f>(D5-E5)/J5</f>
-        <v>5.1515151515151514</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B6" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="20">
-        <v>2</v>
-      </c>
-      <c r="D6" s="59">
-        <v>102</v>
-      </c>
-      <c r="E6" s="55">
-        <v>47.424500000000002</v>
-      </c>
-      <c r="F6" s="20">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G6" s="16">
-        <f t="shared" si="0"/>
-        <v>102</v>
-      </c>
-      <c r="I6">
-        <v>0.2</v>
-      </c>
-      <c r="J6" s="67">
-        <f>E6*I6</f>
-        <v>9.4849000000000014</v>
-      </c>
-      <c r="K6" s="66">
-        <f>E6+3*J6</f>
-        <v>75.879199999999997</v>
-      </c>
-      <c r="L6" s="67">
-        <f>(D6-E6)/J6</f>
-        <v>5.7539352022688686</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B7" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="21">
-        <v>10</v>
-      </c>
-      <c r="D7" s="60">
-        <v>106</v>
-      </c>
-      <c r="E7" s="54">
-        <v>62</v>
-      </c>
-      <c r="F7" s="21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G7" s="18">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="I7">
-        <v>0.13</v>
-      </c>
-      <c r="J7" s="67">
-        <f>E7*I7</f>
-        <v>8.06</v>
-      </c>
-      <c r="K7" s="66">
-        <f>E7+3*J7</f>
-        <v>86.18</v>
-      </c>
-      <c r="L7" s="67">
-        <f>(D7-E7)/J7</f>
-        <v>5.4590570719602978</v>
+        <v>1.2976982759558941E-9</v>
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B9" s="47" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B9" s="50" t="s">
-        <v>41</v>
       </c>
       <c r="C9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" t="s">
-        <v>77</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B10" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B10" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="32" t="s">
+      <c r="E10" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="32" t="s">
+      <c r="H10" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="L10" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="M10" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="N10" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="O10" s="34" t="s">
+      <c r="K10" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="37">
+      <c r="C11" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="34">
         <v>1</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="33">
         <v>1</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="33">
         <v>1</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="34">
         <f>($D$5-$C$5)/D11</f>
-        <v>192</v>
-      </c>
-      <c r="H11" s="36">
+        <v>180</v>
+      </c>
+      <c r="H11" s="33">
         <f>($D$6-$C$6)/E11</f>
         <v>100</v>
       </c>
-      <c r="I11" s="36">
+      <c r="I11" s="33">
         <f>($D$7-$C$7)/F11</f>
-        <v>96</v>
-      </c>
-      <c r="J11" s="40">
+        <v>100</v>
+      </c>
+      <c r="J11" s="37">
         <f>D11/$E$5</f>
         <v>7.575757575757576E-3</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="38">
         <f>E11/$E$6</f>
         <v>2.1086147455429156E-2</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="39">
         <f>F11/$E$7</f>
         <v>1.6129032258064516E-2</v>
       </c>
-      <c r="M11" s="37">
-        <f>($G$5-$F$5)/D11</f>
-        <v>192</v>
-      </c>
-      <c r="N11" s="36">
-        <f>($G$6-$F$6)/E11</f>
-        <v>100</v>
-      </c>
-      <c r="O11" s="36">
-        <f>($G$7-$F$7)/F11</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="20">
+        <v>8</v>
+      </c>
+      <c r="C12" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="17">
         <v>2</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>2</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <v>2</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="17">
         <f>($D$5-$C$5)/D12</f>
-        <v>96</v>
-      </c>
-      <c r="H12" s="15">
+        <v>90</v>
+      </c>
+      <c r="H12" s="14">
         <f>($D$6-$C$6)/E12</f>
         <v>50</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="14">
         <f>($D$7-$C$7)/F12</f>
-        <v>48</v>
-      </c>
-      <c r="J12" s="43">
+        <v>50</v>
+      </c>
+      <c r="J12" s="40">
         <f>D12/$E$5</f>
         <v>1.5151515151515152E-2</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="25">
         <f>E12/$E$6</f>
         <v>4.2172294910858311E-2</v>
       </c>
-      <c r="L12" s="29">
+      <c r="L12" s="26">
         <f>F12/$E$7</f>
         <v>3.2258064516129031E-2</v>
       </c>
-      <c r="M12" s="20">
-        <f>($G$5-$F$5)/D12</f>
-        <v>96</v>
-      </c>
-      <c r="N12" s="15">
-        <f>($G$6-$F$6)/E12</f>
-        <v>50</v>
-      </c>
-      <c r="O12" s="15">
-        <f>($G$7-$F$7)/F12</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="20">
-        <v>4</v>
-      </c>
-      <c r="E13" s="15">
+        <v>11</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="17">
         <v>5</v>
       </c>
-      <c r="F13" s="15">
-        <v>4</v>
-      </c>
-      <c r="G13" s="20">
+      <c r="E13" s="14">
+        <v>5</v>
+      </c>
+      <c r="F13" s="14">
+        <v>5</v>
+      </c>
+      <c r="G13" s="17">
         <f>($D$5-$C$5)/D13</f>
-        <v>48</v>
-      </c>
-      <c r="H13" s="15">
+        <v>36</v>
+      </c>
+      <c r="H13" s="14">
         <f>($D$6-$C$6)/E13</f>
         <v>20</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="14">
         <f>($D$7-$C$7)/F13</f>
-        <v>24</v>
-      </c>
-      <c r="J13" s="43">
+        <v>20</v>
+      </c>
+      <c r="J13" s="40">
         <f>D13/$E$5</f>
-        <v>3.0303030303030304E-2</v>
-      </c>
-      <c r="K13" s="28">
+        <v>3.787878787878788E-2</v>
+      </c>
+      <c r="K13" s="25">
         <f>E13/$E$6</f>
         <v>0.10543073727714578</v>
       </c>
-      <c r="L13" s="29">
+      <c r="L13" s="26">
         <f>F13/$E$7</f>
-        <v>6.4516129032258063E-2</v>
-      </c>
-      <c r="M13" s="20">
-        <f>($G$5-$F$5)/D13</f>
-        <v>48</v>
-      </c>
-      <c r="N13" s="15">
-        <f>($G$6-$F$6)/E13</f>
-        <v>20</v>
-      </c>
-      <c r="O13" s="15">
-        <f>($G$7-$F$7)/F13</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>8.0645161290322578E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="20">
-        <v>12</v>
-      </c>
-      <c r="E14" s="15">
+        <v>32</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="17">
         <v>10</v>
       </c>
-      <c r="F14" s="15">
-        <v>12</v>
-      </c>
-      <c r="G14" s="20">
+      <c r="E14" s="14">
+        <v>10</v>
+      </c>
+      <c r="F14" s="14">
+        <v>10</v>
+      </c>
+      <c r="G14" s="17">
         <f>($D$5-$C$5)/D14</f>
-        <v>16</v>
-      </c>
-      <c r="H14" s="15">
+        <v>18</v>
+      </c>
+      <c r="H14" s="14">
         <f>($D$6-$C$6)/E14</f>
         <v>10</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="14">
         <f>($D$7-$C$7)/F14</f>
-        <v>8</v>
-      </c>
-      <c r="J14" s="43">
+        <v>10</v>
+      </c>
+      <c r="J14" s="40">
         <f>D14/$E$5</f>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="K14" s="28">
+        <v>7.575757575757576E-2</v>
+      </c>
+      <c r="K14" s="25">
         <f>E14/$E$6</f>
         <v>0.21086147455429155</v>
       </c>
-      <c r="L14" s="29">
+      <c r="L14" s="26">
         <f>F14/$E$7</f>
-        <v>0.19354838709677419</v>
-      </c>
-      <c r="M14" s="20">
-        <f>($G$5-$F$5)/D14</f>
-        <v>16</v>
-      </c>
-      <c r="N14" s="15">
-        <f>($G$6-$F$6)/E14</f>
-        <v>10</v>
-      </c>
-      <c r="O14" s="15">
-        <f>($G$7-$F$7)/F14</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+        <v>0.16129032258064516</v>
+      </c>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:15" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="21">
-        <v>24</v>
-      </c>
-      <c r="E15" s="17">
+        <v>54</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="18">
         <v>20</v>
       </c>
-      <c r="F15" s="17">
-        <v>24</v>
-      </c>
-      <c r="G15" s="21">
+      <c r="E15" s="15">
+        <v>20</v>
+      </c>
+      <c r="F15" s="15">
+        <v>20</v>
+      </c>
+      <c r="G15" s="18">
         <f>($D$5-$C$5)/D15</f>
-        <v>8</v>
-      </c>
-      <c r="H15" s="17">
+        <v>9</v>
+      </c>
+      <c r="H15" s="15">
         <f>($D$6-$C$6)/E15</f>
         <v>5</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="15">
         <f>($D$7-$C$7)/F15</f>
-        <v>4</v>
-      </c>
-      <c r="J15" s="44">
+        <v>5</v>
+      </c>
+      <c r="J15" s="41">
         <f>D15/$E$5</f>
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="K15" s="30">
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="K15" s="27">
         <f>E15/$E$6</f>
         <v>0.4217229491085831</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="28">
         <f>F15/$E$7</f>
-        <v>0.38709677419354838</v>
-      </c>
-      <c r="M15" s="21">
-        <f>($G$5-$F$5)/D15</f>
-        <v>8</v>
-      </c>
-      <c r="N15" s="17">
-        <f>($G$6-$F$6)/E15</f>
-        <v>5</v>
-      </c>
-      <c r="O15" s="17">
-        <f>($G$7-$F$7)/F15</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0.32258064516129031</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A17"/>
-      <c r="B17" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="27" t="s">
+      <c r="B17" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+    </row>
+    <row r="18" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B18" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+    </row>
+    <row r="19" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B20" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="1:14" s="2" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.45" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-    </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-    </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-    </row>
-    <row r="22" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
+      <c r="B22" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B24" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="D24" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B25" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="23"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="12" t="s">
+      <c r="C26" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="D26" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.45" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
         <v>28</v>
-      </c>
-      <c r="D26" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -2754,76 +2661,76 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="14.55" x14ac:dyDescent="0.35">
       <c r="D32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="4" t="s">
+    </row>
+    <row r="33" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="D33" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="3" t="s">
+    </row>
+    <row r="34" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B34" s="48">
+        <v>1</v>
+      </c>
+      <c r="C34" s="48" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B34" s="51">
-        <v>1</v>
-      </c>
-      <c r="C34" s="51" t="s">
+      <c r="D34" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52">
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49">
         <v>2</v>
       </c>
-      <c r="H34" s="51">
+      <c r="H34" s="48">
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B35" s="2">
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5">
@@ -2833,19 +2740,19 @@
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B36" s="2">
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G36" s="5">
         <v>2</v>
@@ -2854,37 +2761,37 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B37" s="51">
+    <row r="37" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B37" s="48">
         <v>4</v>
       </c>
-      <c r="C37" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="52" t="s">
+      <c r="C37" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49">
+        <v>2</v>
+      </c>
+      <c r="H37" s="48">
         <v>20</v>
       </c>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52">
-        <v>2</v>
-      </c>
-      <c r="H37" s="51">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B38" s="2">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5">
@@ -2894,19 +2801,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
       <c r="B39" s="2">
         <v>6</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G39" s="5">
         <v>2</v>
@@ -2915,175 +2822,175 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B40" s="51">
+    <row r="40" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B40" s="48">
         <v>7</v>
       </c>
-      <c r="C40" s="51" t="s">
+      <c r="C40" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49">
+        <v>2</v>
+      </c>
+      <c r="H40" s="48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B41" s="48">
+        <v>8</v>
+      </c>
+      <c r="C41" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E40" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52">
+      <c r="D41" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="49">
         <v>2</v>
       </c>
-      <c r="H40" s="51" t="s">
+      <c r="H41" s="48" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="51">
-        <v>8</v>
-      </c>
-      <c r="C41" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="52">
-        <v>2</v>
-      </c>
-      <c r="H41" s="51" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="27" t="s">
-        <v>43</v>
+      <c r="B44" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2">
         <v>0</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2">
         <v>11</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D47" s="64" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2">
         <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D48" s="64"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2">
         <v>13</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" s="64"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2">
         <v>14</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50" s="64"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2">
         <v>15</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D51" s="64"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2">
         <v>21</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D52" s="64" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2">
         <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" s="64"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2">
         <v>23</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" s="64"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2">
         <v>24</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D55" s="64"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2">
         <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D56" s="64"/>
     </row>

</xml_diff>